<commit_message>
First working structure with Advanticsys data
</commit_message>
<xml_diff>
--- a/tests/data/Crop_Growth/Crop_Growth.xlsx
+++ b/tests/data/Crop_Growth/Crop_Growth.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thealanturininstitute-my.sharepoint.com/personal/froumpani_turing_ac_uk/Documents/Turing/2.UrbanAgriculture/Data_original/ExampleData/Synthetic_Data/7-Dat08/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thealanturininstitute-my.sharepoint.com/personal/froumpani_turing_ac_uk/Documents/Turing/2.UrbanAgriculture/CROP/tests/data/Crop_Growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="52" documentId="8_{278B30A4-0CAA-47C5-B766-53DED10BDA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B74C602-3D1D-4351-9528-C9D1DEF89101}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6798816-90B2-4662-A734-1A88D0633FA9}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="624" windowWidth="18180" windowHeight="10932" xr2:uid="{A6798816-90B2-4662-A734-1A88D0633FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="K2" s="13">
         <f ca="1">INT(RAND()*(5-2)+2)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L2" s="14">
         <v>43477</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="P2" s="13">
         <f ca="1">INT(RAND()*(5000-1000)+1000)</f>
-        <v>4798</v>
+        <v>4159</v>
       </c>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
@@ -998,19 +998,19 @@
       <c r="U2" s="16"/>
       <c r="V2" s="13">
         <f ca="1">INT(RAND()*(3000-1000)+1000)</f>
-        <v>2109</v>
+        <v>1734</v>
       </c>
       <c r="W2" s="13">
         <f ca="1">INT(RAND()*(9-1)+1)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="X2" s="13">
         <f ca="1">INT(RAND()*(9-1)+1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y2" s="13">
         <f ca="1">INT(RAND()*(500-50)+50)</f>
-        <v>377</v>
+        <v>205</v>
       </c>
       <c r="Z2" s="17"/>
       <c r="AA2" s="18"/>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="N3" s="13">
         <f t="shared" ref="N3:O21" ca="1" si="1">INT(RAND()*(2-0)+0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="13">
         <f t="shared" ca="1" si="1"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="P3" s="13">
         <f t="shared" ref="P3:P21" ca="1" si="2">INT(RAND()*(5000-1000)+1000)</f>
-        <v>3050</v>
+        <v>2696</v>
       </c>
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
@@ -1080,19 +1080,19 @@
       <c r="U3" s="16"/>
       <c r="V3" s="13">
         <f t="shared" ref="V3:V21" ca="1" si="3">INT(RAND()*(3000-1000)+1000)</f>
-        <v>1079</v>
+        <v>2362</v>
       </c>
       <c r="W3" s="13">
         <f t="shared" ref="W3:X21" ca="1" si="4">INT(RAND()*(9-1)+1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X3" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Y3" s="13">
         <f t="shared" ref="Y3:Y21" ca="1" si="5">INT(RAND()*(500-50)+50)</f>
-        <v>354</v>
+        <v>97</v>
       </c>
       <c r="Z3" s="17"/>
       <c r="AA3" s="18"/>
@@ -1145,15 +1145,15 @@
       </c>
       <c r="N4" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>2961</v>
+        <v>2363</v>
       </c>
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
@@ -1162,19 +1162,19 @@
       <c r="U4" s="16"/>
       <c r="V4" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2304</v>
+        <v>1930</v>
       </c>
       <c r="W4" s="13">
         <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="X4" s="13">
+        <f t="shared" ca="1" si="4"/>
         <v>5</v>
-      </c>
-      <c r="X4" s="13">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
       </c>
       <c r="Y4" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>335</v>
+        <v>198</v>
       </c>
       <c r="Z4" s="17"/>
       <c r="AA4" s="18"/>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="K5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="14">
         <v>43474</v>
@@ -1231,11 +1231,11 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>4498</v>
+        <v>3146</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -1244,7 +1244,7 @@
       <c r="U5" s="16"/>
       <c r="V5" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1745</v>
+        <v>1945</v>
       </c>
       <c r="W5" s="13">
         <f t="shared" ca="1" si="4"/>
@@ -1252,11 +1252,11 @@
       </c>
       <c r="X5" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y5" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="Z5" s="17"/>
       <c r="AA5" s="18"/>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="K6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" s="14">
         <v>43486</v>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="P6" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3634</v>
+        <v>1811</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
@@ -1326,19 +1326,19 @@
       <c r="U6" s="16"/>
       <c r="V6" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2209</v>
+        <v>2319</v>
       </c>
       <c r="W6" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="X6" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18"/>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="K7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L7" s="21">
         <v>43480</v>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="P7" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3902</v>
+        <v>2249</v>
       </c>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
@@ -1408,19 +1408,19 @@
       <c r="U7" s="16"/>
       <c r="V7" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2268</v>
+        <v>2270</v>
       </c>
       <c r="W7" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X7" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y7" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>212</v>
+        <v>485</v>
       </c>
       <c r="Z7" s="17"/>
       <c r="AA7" s="18"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="K8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L8" s="14">
         <v>43479</v>
@@ -1475,15 +1475,15 @@
       </c>
       <c r="N8" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>4898</v>
+        <v>2250</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -1492,19 +1492,19 @@
       <c r="U8" s="16"/>
       <c r="V8" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1849</v>
+        <v>1181</v>
       </c>
       <c r="W8" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X8" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>118</v>
+        <v>359</v>
       </c>
       <c r="Z8" s="17"/>
       <c r="AA8" s="18"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="N9" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="13">
         <f t="shared" ca="1" si="1"/>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="P9" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1988</v>
+        <v>3766</v>
       </c>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
@@ -1574,19 +1574,19 @@
       <c r="U9" s="16"/>
       <c r="V9" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1704</v>
+        <v>2440</v>
       </c>
       <c r="W9" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X9" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Y9" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>283</v>
+        <v>234</v>
       </c>
       <c r="Z9" s="17"/>
       <c r="AA9" s="18"/>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="P10" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3214</v>
+        <v>2550</v>
       </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
@@ -1658,19 +1658,19 @@
       <c r="U10" s="16"/>
       <c r="V10" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1825</v>
+        <v>1974</v>
       </c>
       <c r="W10" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X10" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y10" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>155</v>
+        <v>351</v>
       </c>
       <c r="Z10" s="17"/>
       <c r="AA10" s="18"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="P11" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3036</v>
+        <v>3020</v>
       </c>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
@@ -1740,19 +1740,19 @@
       <c r="U11" s="16"/>
       <c r="V11" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2601</v>
+        <v>1690</v>
       </c>
       <c r="W11" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X11" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>477</v>
+        <v>116</v>
       </c>
       <c r="Z11" s="17"/>
       <c r="AA11" s="18"/>
@@ -1805,15 +1805,15 @@
       </c>
       <c r="N12" s="13">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
-      </c>
-      <c r="O12" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
       </c>
       <c r="P12" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>4008</v>
+        <v>2899</v>
       </c>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
@@ -1822,19 +1822,19 @@
       <c r="U12" s="16"/>
       <c r="V12" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2779</v>
+        <v>2503</v>
       </c>
       <c r="W12" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X12" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y12" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>317</v>
+        <v>407</v>
       </c>
       <c r="Z12" s="17"/>
       <c r="AA12" s="18"/>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="K13" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L13" s="14">
         <v>43474</v>
@@ -1887,15 +1887,15 @@
       </c>
       <c r="N13" s="13">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
-      </c>
-      <c r="O13" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
       </c>
       <c r="P13" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>2675</v>
+        <v>2147</v>
       </c>
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
@@ -1904,11 +1904,11 @@
       <c r="U13" s="16"/>
       <c r="V13" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1682</v>
+        <v>1352</v>
       </c>
       <c r="W13" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X13" s="13">
         <f t="shared" ca="1" si="4"/>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="Y13" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>198</v>
+        <v>320</v>
       </c>
       <c r="Z13" s="17"/>
       <c r="AA13" s="18"/>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="P14" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1232</v>
+        <v>4723</v>
       </c>
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
@@ -1986,19 +1986,19 @@
       <c r="U14" s="16"/>
       <c r="V14" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2053</v>
+        <v>2104</v>
       </c>
       <c r="W14" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X14" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y14" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="Z14" s="17"/>
       <c r="AA14" s="18"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="P15" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>2545</v>
+        <v>3890</v>
       </c>
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
@@ -2070,19 +2070,19 @@
       <c r="U15" s="16"/>
       <c r="V15" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1073</v>
+        <v>2230</v>
       </c>
       <c r="W15" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="X15" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>246</v>
+        <v>399</v>
       </c>
       <c r="Z15" s="17"/>
       <c r="AA15" s="18"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="K16" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L16" s="14">
         <v>43474</v>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P16" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1686</v>
+        <v>4340</v>
       </c>
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
@@ -2152,19 +2152,19 @@
       <c r="U16" s="16"/>
       <c r="V16" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1328</v>
+        <v>2524</v>
       </c>
       <c r="W16" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X16" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Y16" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="Z16" s="17"/>
       <c r="AA16" s="18"/>
@@ -2217,15 +2217,15 @@
       </c>
       <c r="N17" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3215</v>
+        <v>4818</v>
       </c>
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
@@ -2234,19 +2234,19 @@
       <c r="U17" s="16"/>
       <c r="V17" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1121</v>
+        <v>2545</v>
       </c>
       <c r="W17" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X17" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>482</v>
+        <v>182</v>
       </c>
       <c r="Z17" s="17"/>
       <c r="AA17" s="18"/>
@@ -2303,11 +2303,11 @@
       </c>
       <c r="O18" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1717</v>
+        <v>2867</v>
       </c>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
@@ -2316,11 +2316,11 @@
       <c r="U18" s="16"/>
       <c r="V18" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1961</v>
+        <v>2123</v>
       </c>
       <c r="W18" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X18" s="13">
         <f t="shared" ca="1" si="4"/>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="Y18" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="Z18" s="17"/>
       <c r="AA18" s="18"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="K19" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" s="14">
         <v>43474</v>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="N19" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" ca="1" si="1"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="P19" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1960</v>
+        <v>1320</v>
       </c>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
@@ -2398,19 +2398,19 @@
       <c r="U19" s="16"/>
       <c r="V19" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1246</v>
+        <v>1581</v>
       </c>
       <c r="W19" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X19" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Y19" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>481</v>
+        <v>56</v>
       </c>
       <c r="Z19" s="17"/>
       <c r="AA19" s="18"/>
@@ -2467,11 +2467,11 @@
       </c>
       <c r="O20" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3706</v>
+        <v>4021</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
@@ -2480,19 +2480,19 @@
       <c r="U20" s="16"/>
       <c r="V20" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2441</v>
+        <v>2909</v>
       </c>
       <c r="W20" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X20" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Y20" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>368</v>
+        <v>437</v>
       </c>
       <c r="Z20" s="17"/>
       <c r="AA20" s="18"/>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="K21" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L21" s="14">
         <v>43474</v>
@@ -2545,15 +2545,15 @@
       </c>
       <c r="N21" s="13">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
       </c>
       <c r="P21" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>2744</v>
+        <v>4337</v>
       </c>
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
@@ -2562,19 +2562,19 @@
       <c r="U21" s="16"/>
       <c r="V21" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2620</v>
+        <v>2267</v>
       </c>
       <c r="W21" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X21" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y21" s="13">
         <f t="shared" ca="1" si="5"/>
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="Z21" s="17"/>
       <c r="AA21" s="18"/>
@@ -2801,18 +2801,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2835,18 +2835,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353F63CC-E288-49B2-91B4-14FCAC9D04F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80A50077-C8FA-44A9-9978-4EB516DEA64F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353F63CC-E288-49B2-91B4-14FCAC9D04F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>